<commit_message>
Sorting Files, New 35-Det Simulation
</commit_message>
<xml_diff>
--- a/Data/3DetR_cut.xlsx
+++ b/Data/3DetR_cut.xlsx
@@ -616,728 +616,728 @@
     </row>
     <row r="2" spans="1:80">
       <c r="A2">
-        <v>2.458e-05</v>
+        <v>1.96e-06</v>
       </c>
       <c r="B2">
-        <v>2.494e-05</v>
+        <v>2.29e-06</v>
       </c>
       <c r="C2">
-        <v>2.507e-05</v>
+        <v>2.55e-06</v>
       </c>
       <c r="D2">
-        <v>2.46e-05</v>
+        <v>2e-06</v>
       </c>
       <c r="E2">
-        <v>2.703e-05</v>
+        <v>2.07e-06</v>
       </c>
       <c r="F2">
-        <v>2.733e-05</v>
+        <v>2.48e-06</v>
       </c>
       <c r="G2">
-        <v>2.73e-05</v>
+        <v>2.61e-06</v>
       </c>
       <c r="H2">
-        <v>2.828e-05</v>
+        <v>2.85e-06</v>
       </c>
       <c r="I2">
-        <v>2.829e-05</v>
+        <v>2.86e-06</v>
       </c>
       <c r="J2">
-        <v>2.817e-05</v>
+        <v>2.37e-06</v>
       </c>
       <c r="K2">
-        <v>2.758e-05</v>
+        <v>2.42e-06</v>
       </c>
       <c r="L2">
-        <v>2.679e-05</v>
+        <v>1.96e-06</v>
       </c>
       <c r="M2">
-        <v>2.927e-05</v>
+        <v>2.39e-06</v>
       </c>
       <c r="N2">
-        <v>3.034e-05</v>
+        <v>2.97e-06</v>
       </c>
       <c r="O2">
-        <v>3.237e-05</v>
+        <v>3.03e-06</v>
       </c>
       <c r="P2">
-        <v>3.4e-05</v>
+        <v>3.6e-06</v>
       </c>
       <c r="Q2">
-        <v>3.369e-05</v>
+        <v>3.64e-06</v>
       </c>
       <c r="R2">
-        <v>3.2e-05</v>
+        <v>3.12e-06</v>
       </c>
       <c r="S2">
-        <v>3.133e-05</v>
+        <v>2.93e-06</v>
       </c>
       <c r="T2">
-        <v>2.994e-05</v>
+        <v>2.83e-06</v>
       </c>
       <c r="U2">
-        <v>3.276e-05</v>
+        <v>2.56e-06</v>
       </c>
       <c r="V2">
-        <v>3.454e-05</v>
+        <v>3.39e-06</v>
       </c>
       <c r="W2">
-        <v>3.66e-05</v>
+        <v>3.77e-06</v>
       </c>
       <c r="X2">
-        <v>4.054e-05</v>
+        <v>3.91e-06</v>
       </c>
       <c r="Y2">
-        <v>4.189e-05</v>
+        <v>4.65e-06</v>
       </c>
       <c r="Z2">
-        <v>4.212e-05</v>
+        <v>4.24e-06</v>
       </c>
       <c r="AA2">
-        <v>4.063e-05</v>
+        <v>4.17e-06</v>
       </c>
       <c r="AB2">
-        <v>3.779e-05</v>
+        <v>3.7e-06</v>
       </c>
       <c r="AC2">
-        <v>3.504e-05</v>
+        <v>3.33e-06</v>
       </c>
       <c r="AD2">
-        <v>3.457e-05</v>
+        <v>2.79e-06</v>
       </c>
       <c r="AE2">
-        <v>3.802e-05</v>
+        <v>3.67e-06</v>
       </c>
       <c r="AF2">
-        <v>4.285e-05</v>
+        <v>4.41e-06</v>
       </c>
       <c r="AG2">
-        <v>4.798e-05</v>
+        <v>4.82e-06</v>
       </c>
       <c r="AH2">
-        <v>5.145e-05</v>
+        <v>5.6e-06</v>
       </c>
       <c r="AI2">
-        <v>5.543e-05</v>
+        <v>5.96e-06</v>
       </c>
       <c r="AJ2">
-        <v>5.512e-05</v>
+        <v>5.68e-06</v>
       </c>
       <c r="AK2">
-        <v>5.255e-05</v>
+        <v>5.6e-06</v>
       </c>
       <c r="AL2">
-        <v>4.784e-05</v>
+        <v>4.63e-06</v>
       </c>
       <c r="AM2">
-        <v>4.274e-05</v>
+        <v>4.03e-06</v>
       </c>
       <c r="AN2">
-        <v>3.976e-05</v>
+        <v>3.73e-06</v>
       </c>
       <c r="AO2">
-        <v>4.603e-05</v>
+        <v>4.22e-06</v>
       </c>
       <c r="AP2">
-        <v>5.3e-05</v>
+        <v>5.4e-06</v>
       </c>
       <c r="AQ2">
-        <v>6.345e-05</v>
+        <v>6.64e-06</v>
       </c>
       <c r="AR2">
-        <v>7.192e-05</v>
+        <v>7.53e-06</v>
       </c>
       <c r="AS2">
-        <v>7.763e-05</v>
+        <v>8.54e-06</v>
       </c>
       <c r="AT2">
-        <v>7.867e-05</v>
+        <v>8.569999999999999e-06</v>
       </c>
       <c r="AU2">
-        <v>7.332e-05</v>
+        <v>7.36e-06</v>
       </c>
       <c r="AV2">
-        <v>6.316e-05</v>
+        <v>6.53e-06</v>
       </c>
       <c r="AW2">
-        <v>5.254e-05</v>
+        <v>5.26e-06</v>
       </c>
       <c r="AX2">
-        <v>4.618e-05</v>
+        <v>4.1e-06</v>
       </c>
       <c r="AY2">
-        <v>5.508e-05</v>
+        <v>4.56e-06</v>
       </c>
       <c r="AZ2">
-        <v>6.751e-05</v>
+        <v>6.9e-06</v>
       </c>
       <c r="BA2">
-        <v>8.475e-05</v>
+        <v>8.8e-06</v>
       </c>
       <c r="BB2">
-        <v>0.00010316</v>
+        <v>1.141e-05</v>
       </c>
       <c r="BC2">
-        <v>0.00011718</v>
+        <v>1.264e-05</v>
       </c>
       <c r="BD2">
-        <v>0.00011814</v>
+        <v>1.232e-05</v>
       </c>
       <c r="BE2">
-        <v>0.00010465</v>
+        <v>1.108e-05</v>
       </c>
       <c r="BF2">
-        <v>8.53e-05</v>
+        <v>8.72e-06</v>
       </c>
       <c r="BG2">
-        <v>6.857e-05</v>
+        <v>6.86e-06</v>
       </c>
       <c r="BH2">
-        <v>5.625e-05</v>
+        <v>5.13e-06</v>
       </c>
       <c r="BI2">
-        <v>8.53e-05</v>
+        <v>7.93e-06</v>
       </c>
       <c r="BJ2">
-        <v>0.00011753</v>
+        <v>1.233e-05</v>
       </c>
       <c r="BK2">
-        <v>0.00016355</v>
+        <v>1.767e-05</v>
       </c>
       <c r="BL2">
-        <v>0.00020187</v>
+        <v>2.257e-05</v>
       </c>
       <c r="BM2">
-        <v>0.00020352</v>
+        <v>2.201e-05</v>
       </c>
       <c r="BN2">
-        <v>0.00016345</v>
+        <v>1.787e-05</v>
       </c>
       <c r="BO2">
-        <v>0.00011964</v>
+        <v>1.274e-05</v>
       </c>
       <c r="BP2">
-        <v>8.517e-05</v>
+        <v>8.89e-06</v>
       </c>
       <c r="BQ2">
-        <v>8.457e-05</v>
+        <v>7.31e-06</v>
       </c>
       <c r="BR2">
-        <v>0.00016809</v>
+        <v>1.604e-05</v>
       </c>
       <c r="BS2">
-        <v>0.00028123</v>
+        <v>2.956e-05</v>
       </c>
       <c r="BT2">
-        <v>0.00042486</v>
+        <v>4.685e-05</v>
       </c>
       <c r="BU2">
-        <v>0.00042562</v>
+        <v>4.764e-05</v>
       </c>
       <c r="BV2">
-        <v>0.00028523</v>
+        <v>3.053e-05</v>
       </c>
       <c r="BW2">
-        <v>0.00016764</v>
+        <v>1.708e-05</v>
       </c>
       <c r="BX2">
-        <v>8.281e-05</v>
+        <v>7.37e-06</v>
       </c>
       <c r="BY2">
-        <v>0.00050277</v>
+        <v>4.958e-05</v>
       </c>
       <c r="BZ2">
-        <v>0.00134818</v>
+        <v>0.00014724</v>
       </c>
       <c r="CA2">
-        <v>0.00134897</v>
+        <v>0.00014684</v>
       </c>
       <c r="CB2">
-        <v>0.00050339</v>
+        <v>4.951e-05</v>
       </c>
     </row>
     <row r="3" spans="1:80">
       <c r="A3">
-        <v>3.593e-05</v>
+        <v>2.81e-06</v>
       </c>
       <c r="B3">
-        <v>3.125e-05</v>
+        <v>2.87e-06</v>
       </c>
       <c r="C3">
-        <v>2.855e-05</v>
+        <v>2.25e-06</v>
       </c>
       <c r="D3">
-        <v>2.782e-05</v>
+        <v>2.41e-06</v>
       </c>
       <c r="E3">
-        <v>4.935e-05</v>
+        <v>4.51e-06</v>
       </c>
       <c r="F3">
-        <v>4.494e-05</v>
+        <v>4.24e-06</v>
       </c>
       <c r="G3">
-        <v>4.148e-05</v>
+        <v>3.97e-06</v>
       </c>
       <c r="H3">
-        <v>3.615e-05</v>
+        <v>3.61e-06</v>
       </c>
       <c r="I3">
-        <v>3.257e-05</v>
+        <v>2.93e-06</v>
       </c>
       <c r="J3">
-        <v>2.742e-05</v>
+        <v>2.32e-06</v>
       </c>
       <c r="K3">
-        <v>2.569e-05</v>
+        <v>2.37e-06</v>
       </c>
       <c r="L3">
-        <v>2.378e-05</v>
+        <v>1.92e-06</v>
       </c>
       <c r="M3">
-        <v>6.53e-05</v>
+        <v>6.62e-06</v>
       </c>
       <c r="N3">
-        <v>5.847e-05</v>
+        <v>6.06e-06</v>
       </c>
       <c r="O3">
-        <v>5.157e-05</v>
+        <v>5.62e-06</v>
       </c>
       <c r="P3">
-        <v>4.532e-05</v>
+        <v>4.45e-06</v>
       </c>
       <c r="Q3">
-        <v>3.644e-05</v>
+        <v>3.65e-06</v>
       </c>
       <c r="R3">
-        <v>3.214e-05</v>
+        <v>3.25e-06</v>
       </c>
       <c r="S3">
-        <v>2.826e-05</v>
+        <v>2.72e-06</v>
       </c>
       <c r="T3">
-        <v>2.535e-05</v>
+        <v>2.77e-06</v>
       </c>
       <c r="U3">
-        <v>9.564e-05</v>
+        <v>9.57e-06</v>
       </c>
       <c r="V3">
-        <v>9.224e-05</v>
+        <v>9.470000000000001e-06</v>
       </c>
       <c r="W3">
-        <v>8.147e-05</v>
+        <v>8.48e-06</v>
       </c>
       <c r="X3">
-        <v>6.879e-05</v>
+        <v>7.19e-06</v>
       </c>
       <c r="Y3">
-        <v>5.348e-05</v>
+        <v>5.56e-06</v>
       </c>
       <c r="Z3">
-        <v>4.524e-05</v>
+        <v>5.04e-06</v>
       </c>
       <c r="AA3">
-        <v>3.673e-05</v>
+        <v>4.02e-06</v>
       </c>
       <c r="AB3">
-        <v>3e-05</v>
+        <v>2.89e-06</v>
       </c>
       <c r="AC3">
-        <v>2.61e-05</v>
+        <v>2.19e-06</v>
       </c>
       <c r="AD3">
-        <v>2.405e-05</v>
+        <v>2.26e-06</v>
       </c>
       <c r="AE3">
-        <v>0.00015575</v>
+        <v>1.635e-05</v>
       </c>
       <c r="AF3">
-        <v>0.00014867</v>
+        <v>1.586e-05</v>
       </c>
       <c r="AG3">
-        <v>0.000121</v>
+        <v>1.248e-05</v>
       </c>
       <c r="AH3">
-        <v>9.060000000000001e-05</v>
+        <v>9.969999999999999e-06</v>
       </c>
       <c r="AI3">
-        <v>6.79e-05</v>
+        <v>7.43e-06</v>
       </c>
       <c r="AJ3">
-        <v>5.205e-05</v>
+        <v>5.71e-06</v>
       </c>
       <c r="AK3">
-        <v>4.139e-05</v>
+        <v>4.21e-06</v>
       </c>
       <c r="AL3">
-        <v>3.305e-05</v>
+        <v>3.18e-06</v>
       </c>
       <c r="AM3">
-        <v>2.839e-05</v>
+        <v>2.67e-06</v>
       </c>
       <c r="AN3">
-        <v>2.514e-05</v>
+        <v>2.37e-06</v>
       </c>
       <c r="AO3">
-        <v>0.00031931</v>
+        <v>3.339e-05</v>
       </c>
       <c r="AP3">
-        <v>0.00026608</v>
+        <v>2.968e-05</v>
       </c>
       <c r="AQ3">
-        <v>0.00018174</v>
+        <v>2.072e-05</v>
       </c>
       <c r="AR3">
-        <v>0.00012268</v>
+        <v>1.329e-05</v>
       </c>
       <c r="AS3">
-        <v>8.398000000000001e-05</v>
+        <v>9.670000000000001e-06</v>
       </c>
       <c r="AT3">
-        <v>6.063e-05</v>
+        <v>6.25e-06</v>
       </c>
       <c r="AU3">
-        <v>4.595e-05</v>
+        <v>4.88e-06</v>
       </c>
       <c r="AV3">
-        <v>3.758e-05</v>
+        <v>3.96e-06</v>
       </c>
       <c r="AW3">
-        <v>3.048e-05</v>
+        <v>2.93e-06</v>
       </c>
       <c r="AX3">
-        <v>2.648e-05</v>
+        <v>2.25e-06</v>
       </c>
       <c r="AY3">
-        <v>0.00099982</v>
+        <v>0.00010309</v>
       </c>
       <c r="AZ3">
-        <v>0.0005569699999999999</v>
+        <v>6.154e-05</v>
       </c>
       <c r="BA3">
-        <v>0.00027548</v>
+        <v>3.04e-05</v>
       </c>
       <c r="BB3">
-        <v>0.00015535</v>
+        <v>1.668e-05</v>
       </c>
       <c r="BC3">
-        <v>9.795e-05</v>
+        <v>1.095e-05</v>
       </c>
       <c r="BD3">
-        <v>6.654e-05</v>
+        <v>7.1e-06</v>
       </c>
       <c r="BE3">
-        <v>4.854e-05</v>
+        <v>4.97e-06</v>
       </c>
       <c r="BF3">
-        <v>3.813e-05</v>
+        <v>3.81e-06</v>
       </c>
       <c r="BG3">
-        <v>3.075e-05</v>
+        <v>2.84e-06</v>
       </c>
       <c r="BH3">
-        <v>2.748e-05</v>
+        <v>2.32e-06</v>
       </c>
       <c r="BI3">
-        <v>0.00103104</v>
+        <v>0.00011443</v>
       </c>
       <c r="BJ3">
-        <v>0.00034148</v>
+        <v>3.751e-05</v>
       </c>
       <c r="BK3">
-        <v>0.00017097</v>
+        <v>1.876e-05</v>
       </c>
       <c r="BL3">
-        <v>0.00010392</v>
+        <v>1.099e-05</v>
       </c>
       <c r="BM3">
-        <v>7.008000000000001e-05</v>
+        <v>7.4e-06</v>
       </c>
       <c r="BN3">
-        <v>5.214e-05</v>
+        <v>5.39e-06</v>
       </c>
       <c r="BO3">
-        <v>4.133e-05</v>
+        <v>4.11e-06</v>
       </c>
       <c r="BP3">
-        <v>3.406e-05</v>
+        <v>3.26e-06</v>
       </c>
       <c r="BQ3">
-        <v>0.00079811</v>
+        <v>7.769e-05</v>
       </c>
       <c r="BR3">
-        <v>0.00029886</v>
+        <v>3.074e-05</v>
       </c>
       <c r="BS3">
-        <v>0.00015747</v>
+        <v>1.608e-05</v>
       </c>
       <c r="BT3">
-        <v>9.639e-05</v>
+        <v>9.819999999999999e-06</v>
       </c>
       <c r="BU3">
-        <v>6.668000000000001e-05</v>
+        <v>6.29e-06</v>
       </c>
       <c r="BV3">
-        <v>4.917e-05</v>
+        <v>4.66e-06</v>
       </c>
       <c r="BW3">
-        <v>3.946e-05</v>
+        <v>3.54e-06</v>
       </c>
       <c r="BX3">
-        <v>3.561e-05</v>
+        <v>2.67e-06</v>
       </c>
       <c r="BY3">
-        <v>0.00012108</v>
+        <v>1.204e-05</v>
       </c>
       <c r="BZ3">
-        <v>8.640999999999999e-05</v>
+        <v>8.46e-06</v>
       </c>
       <c r="CA3">
-        <v>6.350999999999999e-05</v>
+        <v>6.09e-06</v>
       </c>
       <c r="CB3">
-        <v>4.941e-05</v>
+        <v>4.05e-06</v>
       </c>
     </row>
     <row r="4" spans="1:80">
       <c r="A4">
-        <v>2.679e-05</v>
+        <v>2.13e-06</v>
       </c>
       <c r="B4">
-        <v>2.914e-05</v>
+        <v>2.43e-06</v>
       </c>
       <c r="C4">
-        <v>3.244e-05</v>
+        <v>2.94e-06</v>
       </c>
       <c r="D4">
-        <v>3.554e-05</v>
+        <v>3.01e-06</v>
       </c>
       <c r="E4">
-        <v>2.448e-05</v>
+        <v>1.95e-06</v>
       </c>
       <c r="F4">
-        <v>2.554e-05</v>
+        <v>2.21e-06</v>
       </c>
       <c r="G4">
-        <v>2.837e-05</v>
+        <v>2.78e-06</v>
       </c>
       <c r="H4">
-        <v>3.258e-05</v>
+        <v>2.75e-06</v>
       </c>
       <c r="I4">
-        <v>3.596e-05</v>
+        <v>3.61e-06</v>
       </c>
       <c r="J4">
-        <v>4.013e-05</v>
+        <v>4.27e-06</v>
       </c>
       <c r="K4">
-        <v>4.535e-05</v>
+        <v>4.54e-06</v>
       </c>
       <c r="L4">
-        <v>4.852e-05</v>
+        <v>4.51e-06</v>
       </c>
       <c r="M4">
-        <v>2.469e-05</v>
+        <v>2.18e-06</v>
       </c>
       <c r="N4">
-        <v>2.701e-05</v>
+        <v>2.54e-06</v>
       </c>
       <c r="O4">
-        <v>3.198e-05</v>
+        <v>2.95e-06</v>
       </c>
       <c r="P4">
-        <v>3.785e-05</v>
+        <v>3.89e-06</v>
       </c>
       <c r="Q4">
-        <v>4.469e-05</v>
+        <v>4.38e-06</v>
       </c>
       <c r="R4">
-        <v>5.171e-05</v>
+        <v>5.24e-06</v>
       </c>
       <c r="S4">
-        <v>5.665e-05</v>
+        <v>5.79e-06</v>
       </c>
       <c r="T4">
-        <v>6.489e-05</v>
+        <v>6.2e-06</v>
       </c>
       <c r="U4">
-        <v>2.439e-05</v>
+        <v>1.83e-06</v>
       </c>
       <c r="V4">
-        <v>2.582e-05</v>
+        <v>2.45e-06</v>
       </c>
       <c r="W4">
-        <v>3.115e-05</v>
+        <v>3.01e-06</v>
       </c>
       <c r="X4">
-        <v>3.722e-05</v>
+        <v>3.91e-06</v>
       </c>
       <c r="Y4">
-        <v>4.436e-05</v>
+        <v>4.43e-06</v>
       </c>
       <c r="Z4">
-        <v>5.535e-05</v>
+        <v>5.66e-06</v>
       </c>
       <c r="AA4">
-        <v>6.642e-05</v>
+        <v>6.82e-06</v>
       </c>
       <c r="AB4">
-        <v>8.1e-05</v>
+        <v>8.81e-06</v>
       </c>
       <c r="AC4">
-        <v>8.988e-05</v>
+        <v>9.079999999999999e-06</v>
       </c>
       <c r="AD4">
-        <v>9.616e-05</v>
+        <v>9.51e-06</v>
       </c>
       <c r="AE4">
-        <v>2.492e-05</v>
+        <v>2.44e-06</v>
       </c>
       <c r="AF4">
-        <v>2.805e-05</v>
+        <v>2.42e-06</v>
       </c>
       <c r="AG4">
-        <v>3.403e-05</v>
+        <v>3.18e-06</v>
       </c>
       <c r="AH4">
-        <v>4.108e-05</v>
+        <v>4.29e-06</v>
       </c>
       <c r="AI4">
-        <v>5.301e-05</v>
+        <v>5.34e-06</v>
       </c>
       <c r="AJ4">
-        <v>6.766999999999999e-05</v>
+        <v>6.93e-06</v>
       </c>
       <c r="AK4">
-        <v>9.055000000000001e-05</v>
+        <v>1.012e-05</v>
       </c>
       <c r="AL4">
-        <v>0.00011833</v>
+        <v>1.242e-05</v>
       </c>
       <c r="AM4">
-        <v>0.00014541</v>
+        <v>1.598e-05</v>
       </c>
       <c r="AN4">
-        <v>0.00015678</v>
+        <v>1.576e-05</v>
       </c>
       <c r="AO4">
-        <v>2.623e-05</v>
+        <v>2.34e-06</v>
       </c>
       <c r="AP4">
-        <v>3.093e-05</v>
+        <v>2.97e-06</v>
       </c>
       <c r="AQ4">
-        <v>3.663e-05</v>
+        <v>3.56e-06</v>
       </c>
       <c r="AR4">
-        <v>4.516e-05</v>
+        <v>4.9e-06</v>
       </c>
       <c r="AS4">
-        <v>6.062e-05</v>
+        <v>6.4e-06</v>
       </c>
       <c r="AT4">
-        <v>8.383e-05</v>
+        <v>9.310000000000001e-06</v>
       </c>
       <c r="AU4">
-        <v>0.00012122</v>
+        <v>1.333e-05</v>
       </c>
       <c r="AV4">
-        <v>0.0001829</v>
+        <v>2.036e-05</v>
       </c>
       <c r="AW4">
-        <v>0.00026762</v>
+        <v>2.916e-05</v>
       </c>
       <c r="AX4">
-        <v>0.0003188</v>
+        <v>3.181e-05</v>
       </c>
       <c r="AY4">
-        <v>2.881e-05</v>
+        <v>2.53e-06</v>
       </c>
       <c r="AZ4">
-        <v>3.214e-05</v>
+        <v>2.96e-06</v>
       </c>
       <c r="BA4">
-        <v>3.813e-05</v>
+        <v>4.07e-06</v>
       </c>
       <c r="BB4">
-        <v>4.934e-05</v>
+        <v>5.08e-06</v>
       </c>
       <c r="BC4">
-        <v>6.69e-05</v>
+        <v>7.42e-06</v>
       </c>
       <c r="BD4">
-        <v>9.619e-05</v>
+        <v>1.004e-05</v>
       </c>
       <c r="BE4">
-        <v>0.00015408</v>
+        <v>1.72e-05</v>
       </c>
       <c r="BF4">
-        <v>0.00027613</v>
+        <v>3.094e-05</v>
       </c>
       <c r="BG4">
-        <v>0.00056178</v>
+        <v>6.211999999999999e-05</v>
       </c>
       <c r="BH4">
-        <v>0.00099664</v>
+        <v>0.0001042</v>
       </c>
       <c r="BI4">
-        <v>3.411e-05</v>
+        <v>2.84e-06</v>
       </c>
       <c r="BJ4">
-        <v>4.123e-05</v>
+        <v>3.87e-06</v>
       </c>
       <c r="BK4">
-        <v>5.114e-05</v>
+        <v>5.27e-06</v>
       </c>
       <c r="BL4">
-        <v>7.001e-05</v>
+        <v>7.37e-06</v>
       </c>
       <c r="BM4">
-        <v>0.0001025</v>
+        <v>1.08e-05</v>
       </c>
       <c r="BN4">
-        <v>0.00017363</v>
+        <v>1.844e-05</v>
       </c>
       <c r="BO4">
-        <v>0.00034591</v>
+        <v>3.827e-05</v>
       </c>
       <c r="BP4">
-        <v>0.00103716</v>
+        <v>0.0001153</v>
       </c>
       <c r="BQ4">
-        <v>3.438e-05</v>
+        <v>2.88e-06</v>
       </c>
       <c r="BR4">
-        <v>3.936e-05</v>
+        <v>4.06e-06</v>
       </c>
       <c r="BS4">
-        <v>4.992e-05</v>
+        <v>5.56e-06</v>
       </c>
       <c r="BT4">
-        <v>6.692e-05</v>
+        <v>6.44e-06</v>
       </c>
       <c r="BU4">
-        <v>9.842e-05</v>
+        <v>9.660000000000001e-06</v>
       </c>
       <c r="BV4">
-        <v>0.00015618</v>
+        <v>1.636e-05</v>
       </c>
       <c r="BW4">
-        <v>0.00029962</v>
+        <v>3.098e-05</v>
       </c>
       <c r="BX4">
-        <v>0.00079604</v>
+        <v>7.872000000000001e-05</v>
       </c>
       <c r="BY4">
-        <v>5.098e-05</v>
+        <v>4.59e-06</v>
       </c>
       <c r="BZ4">
-        <v>6.437e-05</v>
+        <v>6.25e-06</v>
       </c>
       <c r="CA4">
-        <v>8.589000000000001e-05</v>
+        <v>8.080000000000001e-06</v>
       </c>
       <c r="CB4">
-        <v>0.00011923</v>
+        <v>1.139e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>